<commit_message>
caminos del pert COMPLETOS AAAAAAAAAAAAA
</commit_message>
<xml_diff>
--- a/Actividades/Proy01008/Duraciones/Primera entrega pert duraciones.xlsx
+++ b/Actividades/Proy01008/Duraciones/Primera entrega pert duraciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ProyectoFinal2019-\Actividades\Proy01008\Duraciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\HUB\ProyectoFinal2019-\Actividades\Proy01008\Duraciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB68E8C8-BD58-4C16-9019-1CF4A89E86F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6F2A9A-70DC-45B8-BB17-E4CC9C5C8B2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="690" windowWidth="11535" windowHeight="14910" xr2:uid="{1903A301-E6C9-455A-B3A9-39FDA3101E53}"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="10395" windowHeight="14910" xr2:uid="{1903A301-E6C9-455A-B3A9-39FDA3101E53}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>

</xml_diff>